<commit_message>
added the error checking for delay problem
</commit_message>
<xml_diff>
--- a/Measured_data/performance.xlsx
+++ b/Measured_data/performance.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>segLen</t>
   </si>
@@ -33,6 +33,9 @@
   </si>
   <si>
     <t>Up to 100</t>
+  </si>
+  <si>
+    <t>(sec)</t>
   </si>
 </sst>
 </file>
@@ -359,8 +362,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -376,6 +379,9 @@
       </c>
     </row>
     <row r="4" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="C4" s="1">
         <v>0.1</v>
       </c>

</xml_diff>